<commit_message>
messo il controllo sul tipo documento e cancellato le righe con 0 in lett.attuale
</commit_message>
<xml_diff>
--- a/EE_2021-05-31.xlsx
+++ b/EE_2021-05-31.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24931"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25225"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\java\photon2\readfatt\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{31E0EEEB-60DA-4A15-859B-F9089FB3DBBB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A352C0A2-3602-44C1-9A82-EA8ACA4E79F1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-35790" yWindow="345" windowWidth="15720" windowHeight="10245" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-14595" yWindow="150" windowWidth="14520" windowHeight="14685" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="2021-05-31" sheetId="1" r:id="rId1"/>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="27">
   <si>
     <t>Periodo</t>
   </si>
@@ -38,79 +38,79 @@
     <t xml:space="preserve">fattura </t>
   </si>
   <si>
+    <t>Contatore</t>
+  </si>
+  <si>
+    <t>Credito</t>
+  </si>
+  <si>
+    <t>kWh</t>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t>Scagl</t>
+  </si>
+  <si>
+    <t>Costo</t>
+  </si>
+  <si>
+    <t>Rifiuti</t>
+  </si>
+  <si>
+    <t>Tot</t>
+  </si>
+  <si>
+    <t>del</t>
+  </si>
+  <si>
+    <t>1^</t>
+  </si>
+  <si>
+    <t>Tot. Calc</t>
+  </si>
+  <si>
+    <t>2^</t>
+  </si>
+  <si>
+    <t>dt.Lettura Attuale</t>
+  </si>
+  <si>
+    <t>Preced.</t>
+  </si>
+  <si>
+    <t>Attuale</t>
+  </si>
+  <si>
+    <t>Consumo</t>
+  </si>
+  <si>
+    <t>Netto</t>
+  </si>
+  <si>
+    <t>1^Scagl.</t>
+  </si>
+  <si>
+    <t>2^Scagl.</t>
+  </si>
+  <si>
+    <t>Cont.</t>
+  </si>
+  <si>
+    <t>Costo 1</t>
+  </si>
+  <si>
+    <t>Costo 2</t>
+  </si>
+  <si>
+    <t>Energia attiva</t>
+  </si>
+  <si>
+    <t>Totale</t>
+  </si>
+  <si>
     <t>2022/1000885</t>
-  </si>
-  <si>
-    <t>Contatore</t>
-  </si>
-  <si>
-    <t>Credito</t>
-  </si>
-  <si>
-    <t>kWh</t>
-  </si>
-  <si>
-    <t/>
-  </si>
-  <si>
-    <t>Scagl</t>
-  </si>
-  <si>
-    <t>Costo</t>
-  </si>
-  <si>
-    <t>Rifiuti</t>
-  </si>
-  <si>
-    <t>Tot</t>
-  </si>
-  <si>
-    <t>del</t>
-  </si>
-  <si>
-    <t>1^</t>
-  </si>
-  <si>
-    <t>Tot. Calc</t>
-  </si>
-  <si>
-    <t>2^</t>
-  </si>
-  <si>
-    <t>dt.Lettura Attuale</t>
-  </si>
-  <si>
-    <t>Preced.</t>
-  </si>
-  <si>
-    <t>Attuale</t>
-  </si>
-  <si>
-    <t>Consumo</t>
-  </si>
-  <si>
-    <t>Netto</t>
-  </si>
-  <si>
-    <t>1^Scagl.</t>
-  </si>
-  <si>
-    <t>2^Scagl.</t>
-  </si>
-  <si>
-    <t>Cont.</t>
-  </si>
-  <si>
-    <t>Costo 1</t>
-  </si>
-  <si>
-    <t>Costo 2</t>
-  </si>
-  <si>
-    <t>Energia attiva</t>
-  </si>
-  <si>
-    <t>Totale</t>
   </si>
 </sst>
 </file>
@@ -120,7 +120,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.000000"/>
   </numFmts>
-  <fonts count="56" x14ac:knownFonts="1">
+  <fonts count="57" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color indexed="8"/>
@@ -236,6 +236,13 @@
     </font>
     <font>
       <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -677,7 +684,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="56">
+  <cellXfs count="57">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="14" fontId="2" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -708,76 +715,77 @@
     <xf numFmtId="164" fontId="15" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="4" fontId="16" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="14" fontId="17" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="18" fillId="2" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="19" fillId="2" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="20" fillId="2" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="18" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="19" fillId="2" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="20" fillId="2" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="21" fillId="2" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="2" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="22" fillId="2" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="24" fillId="2" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="2" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="25" fillId="2" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="2" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="26" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="27" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="27" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="28" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="14" fontId="28" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="3" fontId="29" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="3" fontId="30" fillId="2" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="31" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="32" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="33" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="2" fontId="34" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="4" fontId="35" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="4" fontId="36" fillId="2" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="14" fontId="37" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="3" fontId="38" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="3" fontId="39" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="3" fontId="40" fillId="2" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="2" fontId="41" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="4" fontId="42" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="4" fontId="43" fillId="2" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="14" fontId="44" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="45" fillId="2" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="46" fillId="2" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="14" fontId="47" fillId="3" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="3" fontId="48" fillId="2" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="3" fontId="49" fillId="3" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="3" fontId="50" fillId="2" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="51" fillId="2" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="2" fontId="52" fillId="2" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="4" fontId="53" fillId="2" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="4" fontId="54" fillId="2" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="4" fontId="55" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="14" fontId="29" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="3" fontId="30" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="3" fontId="31" fillId="2" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="32" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="33" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="34" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="35" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="4" fontId="36" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="4" fontId="37" fillId="2" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="14" fontId="38" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="3" fontId="39" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="3" fontId="40" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="3" fontId="41" fillId="2" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="2" fontId="42" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="4" fontId="43" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="4" fontId="44" fillId="2" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="14" fontId="45" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="46" fillId="2" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="47" fillId="2" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="14" fontId="48" fillId="3" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="3" fontId="49" fillId="2" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="3" fontId="50" fillId="3" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="3" fontId="51" fillId="2" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="52" fillId="2" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="2" fontId="53" fillId="2" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="4" fontId="54" fillId="2" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="4" fontId="55" fillId="2" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="4" fontId="56" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normale" xfId="0" builtinId="0"/>
@@ -1092,10 +1100,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:N11"/>
+  <dimension ref="A1:N12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:XFD1048576"/>
+      <selection activeCell="B6" sqref="B6:N9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1127,42 +1135,42 @@
         <v>1</v>
       </c>
       <c r="E1" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="F1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="H1" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="H1" s="4" t="s">
+      <c r="I1" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="I1" s="4" t="s">
-        <v>5</v>
-      </c>
       <c r="J1" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="K1" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="K1" s="6" t="s">
+      <c r="L1" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="L1" s="7" t="s">
+      <c r="N1" s="8" t="s">
         <v>8</v>
-      </c>
-      <c r="N1" s="8" t="s">
-        <v>9</v>
       </c>
     </row>
     <row r="2" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B2" s="9">
         <v>174.89</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="E2" s="2">
-        <v>44589</v>
+        <v>21024</v>
       </c>
       <c r="F2" s="10">
         <v>4.5</v>
@@ -1171,10 +1179,10 @@
         <v>2020</v>
       </c>
       <c r="I2" s="11">
-        <v>633</v>
+        <v>0</v>
       </c>
       <c r="J2" s="12" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="K2" s="13">
         <v>163</v>
@@ -1188,29 +1196,29 @@
     </row>
     <row r="3" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B3" s="16">
+        <f>K12+L12+M12+N12</f>
+        <v>283.72520000000003</v>
+      </c>
+      <c r="D3" s="17" t="s">
+        <v>5</v>
+      </c>
+      <c r="E3" s="17" t="s">
+        <v>5</v>
+      </c>
+      <c r="F3" s="17" t="s">
+        <v>5</v>
+      </c>
+      <c r="H3" s="11">
+        <v>0</v>
+      </c>
+      <c r="I3" s="11">
+        <v>0</v>
+      </c>
+      <c r="J3" s="12" t="s">
         <v>13</v>
-      </c>
-      <c r="B3" s="16">
-        <f>K11+L11+M11+N11</f>
-        <v>196.38493000000003</v>
-      </c>
-      <c r="D3" s="17" t="s">
-        <v>6</v>
-      </c>
-      <c r="E3" s="17" t="s">
-        <v>6</v>
-      </c>
-      <c r="F3" s="17" t="s">
-        <v>6</v>
-      </c>
-      <c r="H3" s="11">
-        <v>2020</v>
-      </c>
-      <c r="I3" s="11">
-        <v>0</v>
-      </c>
-      <c r="J3" s="12" t="s">
-        <v>14</v>
       </c>
       <c r="K3" s="13">
         <v>300</v>
@@ -1219,185 +1227,160 @@
         <v>0.18951000000000001</v>
       </c>
     </row>
-    <row r="4" spans="1:14" ht="30" x14ac:dyDescent="0.25">
-      <c r="A4" s="18" t="s">
-        <v>6</v>
-      </c>
-      <c r="B4" s="19" t="s">
-        <v>6</v>
-      </c>
-      <c r="C4" s="20" t="s">
+    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="B4" s="16" t="s">
+        <v>5</v>
+      </c>
+      <c r="D4" s="17" t="s">
+        <v>5</v>
+      </c>
+      <c r="E4" s="17" t="s">
+        <v>5</v>
+      </c>
+      <c r="F4" s="17" t="s">
+        <v>5</v>
+      </c>
+      <c r="H4" s="11">
+        <v>0</v>
+      </c>
+      <c r="I4" s="11">
+        <v>0</v>
+      </c>
+      <c r="J4" s="13" t="s">
+        <v>5</v>
+      </c>
+      <c r="K4" s="13" t="s">
+        <v>5</v>
+      </c>
+      <c r="L4" s="18" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="5" spans="1:14" ht="30" x14ac:dyDescent="0.25">
+      <c r="A5" s="19" t="s">
+        <v>5</v>
+      </c>
+      <c r="B5" s="20" t="s">
+        <v>5</v>
+      </c>
+      <c r="C5" s="21" t="s">
+        <v>14</v>
+      </c>
+      <c r="D5" s="22" t="s">
         <v>15</v>
       </c>
-      <c r="D4" s="21" t="s">
+      <c r="E5" s="22" t="s">
         <v>16</v>
       </c>
-      <c r="E4" s="21" t="s">
+      <c r="F5" s="7" t="s">
         <v>17</v>
       </c>
-      <c r="F4" s="7" t="s">
+      <c r="G5" s="23" t="s">
+        <v>3</v>
+      </c>
+      <c r="H5" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="G4" s="22" t="s">
-        <v>4</v>
-      </c>
-      <c r="H4" s="5" t="s">
+      <c r="I5" s="6" t="s">
         <v>19</v>
       </c>
-      <c r="I4" s="6" t="s">
+      <c r="J5" s="24" t="s">
         <v>20</v>
       </c>
-      <c r="J4" s="23" t="s">
+      <c r="K5" s="24" t="s">
         <v>21</v>
       </c>
-      <c r="K4" s="23" t="s">
+      <c r="L5" s="24" t="s">
         <v>22</v>
       </c>
-      <c r="L4" s="23" t="s">
+      <c r="M5" s="25" t="s">
         <v>23</v>
       </c>
-      <c r="M4" s="24" t="s">
+      <c r="N5" s="26" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="6" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A6" s="27" t="s">
         <v>24</v>
       </c>
-      <c r="N4" s="25" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A5" s="26" t="s">
-        <v>25</v>
-      </c>
-      <c r="B5" s="27" t="s">
-        <v>6</v>
-      </c>
-      <c r="C5" s="28">
+      <c r="B6" s="28" t="s">
+        <v>5</v>
+      </c>
+      <c r="C6" s="29">
         <v>44347</v>
       </c>
-      <c r="D5" s="29">
+      <c r="D6" s="30">
         <v>24879</v>
       </c>
-      <c r="E5" s="29">
+      <c r="E6" s="30">
         <v>25173</v>
       </c>
-      <c r="F5" s="30">
-        <f>IF(E5-D5&gt;0,E5-D5,0)</f>
+      <c r="F6" s="31">
+        <f>IF(E6-D6&gt;0,E6-D6,0)</f>
         <v>294</v>
       </c>
-      <c r="G5" s="13">
+      <c r="G6" s="13">
         <f>I2</f>
-        <v>633</v>
-      </c>
-      <c r="H5" s="31">
-        <f>IF(F5-G5&gt;0,F5-G5,0)</f>
-        <v>0</v>
-      </c>
-      <c r="I5" s="32">
-        <f>IF(H5&lt;$K$2,H5,$K$2)</f>
-        <v>0</v>
-      </c>
-      <c r="J5" s="33">
-        <f>H5-I5</f>
-        <v>0</v>
-      </c>
-      <c r="K5" s="34">
+        <v>0</v>
+      </c>
+      <c r="H6" s="32">
+        <f>IF(F6-G6&gt;0,F6-G6,0)</f>
+        <v>294</v>
+      </c>
+      <c r="I6" s="33">
+        <f>IF(H6&lt;$K$2,H6,$K$2)</f>
+        <v>163</v>
+      </c>
+      <c r="J6" s="34">
+        <f>H6-I6</f>
+        <v>131</v>
+      </c>
+      <c r="K6" s="35">
         <f>$F$2</f>
         <v>4.5</v>
       </c>
-      <c r="L5" s="35">
-        <f>I5*$L$2</f>
-        <v>0</v>
-      </c>
-      <c r="M5" s="35">
-        <f>J5*$L$3</f>
-        <v>0</v>
-      </c>
-      <c r="N5" s="36">
-        <f>F5*$N$2</f>
+      <c r="L6" s="36">
+        <f>I6*$L$2</f>
+        <v>14.580350000000001</v>
+      </c>
+      <c r="M6" s="36">
+        <f>J6*$L$3</f>
+        <v>24.825810000000001</v>
+      </c>
+      <c r="N6" s="37">
+        <f>F6*$N$2</f>
         <v>17.384219999999999</v>
-      </c>
-    </row>
-    <row r="6" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A6" s="12" t="s">
-        <v>6</v>
-      </c>
-      <c r="B6" s="13" t="s">
-        <v>6</v>
-      </c>
-      <c r="C6" s="37">
-        <v>44377</v>
-      </c>
-      <c r="D6" s="38">
-        <f>E5</f>
-        <v>25173</v>
-      </c>
-      <c r="E6" s="39">
-        <v>25477</v>
-      </c>
-      <c r="F6" s="40">
-        <f>IF(E6-D6&gt;0,E6-D6,0)</f>
-        <v>304</v>
-      </c>
-      <c r="G6" s="13">
-        <f>IF(G5-F5&gt;0,G5-F5,0)</f>
-        <v>339</v>
-      </c>
-      <c r="H6" s="12">
-        <f>IF(F6-G6&gt;0,F6-G6,0)</f>
-        <v>0</v>
-      </c>
-      <c r="I6" s="8">
-        <f>IF(H6&lt;$K$2,H6,$K$2)</f>
-        <v>0</v>
-      </c>
-      <c r="J6" s="13">
-        <f>H6-I6</f>
-        <v>0</v>
-      </c>
-      <c r="K6" s="41">
-        <f>$F$2</f>
-        <v>4.5</v>
-      </c>
-      <c r="L6" s="42">
-        <f>I6*$L$2</f>
-        <v>0</v>
-      </c>
-      <c r="M6" s="42">
-        <f>J6*$L$3</f>
-        <v>0</v>
-      </c>
-      <c r="N6" s="43">
-        <f>F6*$N$2</f>
-        <v>17.975519999999999</v>
       </c>
     </row>
     <row r="7" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A7" s="12" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B7" s="13" t="s">
-        <v>6</v>
-      </c>
-      <c r="C7" s="44">
-        <v>44408</v>
-      </c>
-      <c r="D7" s="38">
+        <v>5</v>
+      </c>
+      <c r="C7" s="38">
+        <v>44377</v>
+      </c>
+      <c r="D7" s="39">
         <f>E6</f>
+        <v>25173</v>
+      </c>
+      <c r="E7" s="40">
         <v>25477</v>
       </c>
-      <c r="E7" s="39">
-        <v>25831</v>
-      </c>
-      <c r="F7" s="40">
+      <c r="F7" s="41">
         <f>IF(E7-D7&gt;0,E7-D7,0)</f>
-        <v>354</v>
+        <v>304</v>
       </c>
       <c r="G7" s="13">
         <f>IF(G6-F6&gt;0,G6-F6,0)</f>
-        <v>35</v>
+        <v>0</v>
       </c>
       <c r="H7" s="12">
         <f>IF(F7-G7&gt;0,F7-G7,0)</f>
-        <v>319</v>
+        <v>304</v>
       </c>
       <c r="I7" s="8">
         <f>IF(H7&lt;$K$2,H7,$K$2)</f>
@@ -1405,45 +1388,45 @@
       </c>
       <c r="J7" s="13">
         <f>H7-I7</f>
-        <v>156</v>
-      </c>
-      <c r="K7" s="41">
+        <v>141</v>
+      </c>
+      <c r="K7" s="42">
         <f>$F$2</f>
         <v>4.5</v>
       </c>
-      <c r="L7" s="42">
+      <c r="L7" s="43">
         <f>I7*$L$2</f>
         <v>14.580350000000001</v>
       </c>
-      <c r="M7" s="42">
+      <c r="M7" s="43">
         <f>J7*$L$3</f>
-        <v>29.563560000000003</v>
-      </c>
-      <c r="N7" s="43">
+        <v>26.72091</v>
+      </c>
+      <c r="N7" s="44">
         <f>F7*$N$2</f>
-        <v>20.932020000000001</v>
+        <v>17.975519999999999</v>
       </c>
     </row>
     <row r="8" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A8" s="12" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B8" s="13" t="s">
-        <v>6</v>
-      </c>
-      <c r="C8" s="37">
-        <v>44439</v>
-      </c>
-      <c r="D8" s="38">
+        <v>5</v>
+      </c>
+      <c r="C8" s="45">
+        <v>44408</v>
+      </c>
+      <c r="D8" s="39">
         <f>E7</f>
+        <v>25477</v>
+      </c>
+      <c r="E8" s="40">
         <v>25831</v>
       </c>
-      <c r="E8" s="39">
-        <v>26192</v>
-      </c>
-      <c r="F8" s="40">
+      <c r="F8" s="41">
         <f>IF(E8-D8&gt;0,E8-D8,0)</f>
-        <v>361</v>
+        <v>354</v>
       </c>
       <c r="G8" s="13">
         <f>IF(G7-F7&gt;0,G7-F7,0)</f>
@@ -1451,7 +1434,7 @@
       </c>
       <c r="H8" s="12">
         <f>IF(F8-G8&gt;0,F8-G8,0)</f>
-        <v>361</v>
+        <v>354</v>
       </c>
       <c r="I8" s="8">
         <f>IF(H8&lt;$K$2,H8,$K$2)</f>
@@ -1459,97 +1442,151 @@
       </c>
       <c r="J8" s="13">
         <f>H8-I8</f>
-        <v>198</v>
-      </c>
-      <c r="K8" s="41">
+        <v>191</v>
+      </c>
+      <c r="K8" s="42">
         <f>$F$2</f>
         <v>4.5</v>
       </c>
-      <c r="L8" s="42">
+      <c r="L8" s="43">
         <f>I8*$L$2</f>
         <v>14.580350000000001</v>
       </c>
-      <c r="M8" s="42">
+      <c r="M8" s="43">
         <f>J8*$L$3</f>
-        <v>37.522980000000004</v>
-      </c>
-      <c r="N8" s="43">
+        <v>36.19641</v>
+      </c>
+      <c r="N8" s="44">
         <f>F8*$N$2</f>
-        <v>21.345929999999999</v>
+        <v>20.932020000000001</v>
       </c>
     </row>
     <row r="9" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A9" s="45" t="s">
-        <v>6</v>
-      </c>
-      <c r="B9" s="46" t="s">
-        <v>6</v>
-      </c>
-      <c r="C9" s="47">
+      <c r="A9" s="12" t="s">
+        <v>5</v>
+      </c>
+      <c r="B9" s="13" t="s">
+        <v>5</v>
+      </c>
+      <c r="C9" s="38">
         <v>44439</v>
       </c>
-      <c r="D9" s="48">
+      <c r="D9" s="39">
         <f>E8</f>
+        <v>25831</v>
+      </c>
+      <c r="E9" s="40">
         <v>26192</v>
       </c>
-      <c r="E9" s="49">
-        <v>0</v>
-      </c>
-      <c r="F9" s="50">
+      <c r="F9" s="41">
         <f>IF(E9-D9&gt;0,E9-D9,0)</f>
-        <v>0</v>
+        <v>361</v>
       </c>
       <c r="G9" s="13">
         <f>IF(G8-F8&gt;0,G8-F8,0)</f>
         <v>0</v>
       </c>
-      <c r="H9" s="45">
+      <c r="H9" s="12">
         <f>IF(F9-G9&gt;0,F9-G9,0)</f>
-        <v>0</v>
-      </c>
-      <c r="I9" s="51">
+        <v>361</v>
+      </c>
+      <c r="I9" s="8">
         <f>IF(H9&lt;$K$2,H9,$K$2)</f>
-        <v>0</v>
-      </c>
-      <c r="J9" s="46">
+        <v>163</v>
+      </c>
+      <c r="J9" s="13">
         <f>H9-I9</f>
-        <v>0</v>
-      </c>
-      <c r="K9" s="52">
+        <v>198</v>
+      </c>
+      <c r="K9" s="42">
         <f>$F$2</f>
         <v>4.5</v>
       </c>
-      <c r="L9" s="53">
+      <c r="L9" s="43">
         <f>I9*$L$2</f>
-        <v>0</v>
-      </c>
-      <c r="M9" s="53">
+        <v>14.580350000000001</v>
+      </c>
+      <c r="M9" s="43">
         <f>J9*$L$3</f>
-        <v>0</v>
-      </c>
-      <c r="N9" s="54">
+        <v>37.522980000000004</v>
+      </c>
+      <c r="N9" s="44">
         <f>F9*$N$2</f>
-        <v>0</v>
+        <v>21.345929999999999</v>
       </c>
     </row>
-    <row r="11" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="J11" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="K11" s="55">
-        <f>SUM(K5:K9)</f>
+    <row r="10" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A10" s="46" t="s">
+        <v>5</v>
+      </c>
+      <c r="B10" s="47" t="s">
+        <v>5</v>
+      </c>
+      <c r="C10" s="48">
+        <v>44439</v>
+      </c>
+      <c r="D10" s="49">
+        <f>E9</f>
+        <v>26192</v>
+      </c>
+      <c r="E10" s="50">
+        <v>0</v>
+      </c>
+      <c r="F10" s="51">
+        <f>IF(E10-D10&gt;0,E10-D10,0)</f>
+        <v>0</v>
+      </c>
+      <c r="G10" s="13">
+        <f>IF(G9-F9&gt;0,G9-F9,0)</f>
+        <v>0</v>
+      </c>
+      <c r="H10" s="46">
+        <f>IF(F10-G10&gt;0,F10-G10,0)</f>
+        <v>0</v>
+      </c>
+      <c r="I10" s="52">
+        <f>IF(H10&lt;$K$2,H10,$K$2)</f>
+        <v>0</v>
+      </c>
+      <c r="J10" s="47">
+        <f>H10-I10</f>
+        <v>0</v>
+      </c>
+      <c r="K10" s="53">
+        <f>$F$2</f>
+        <v>4.5</v>
+      </c>
+      <c r="L10" s="54">
+        <f>I10*$L$2</f>
+        <v>0</v>
+      </c>
+      <c r="M10" s="54">
+        <f>J10*$L$3</f>
+        <v>0</v>
+      </c>
+      <c r="N10" s="55">
+        <f>F10*$N$2</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="J12" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="K12" s="56">
+        <f>SUM(K6:K10)</f>
         <v>22.5</v>
       </c>
-      <c r="L11" s="55">
-        <f>SUM(L5:L9)</f>
-        <v>29.160700000000002</v>
-      </c>
-      <c r="M11" s="55">
-        <f>SUM(M5:M9)</f>
-        <v>67.086540000000014</v>
-      </c>
-      <c r="N11" s="55">
-        <f>SUM(N5:N9)</f>
+      <c r="L12" s="56">
+        <f>SUM(L6:L10)</f>
+        <v>58.321400000000004</v>
+      </c>
+      <c r="M12" s="56">
+        <f>SUM(M6:M10)</f>
+        <v>125.26611000000001</v>
+      </c>
+      <c r="N12" s="56">
+        <f>SUM(N6:N10)</f>
         <v>77.637690000000006</v>
       </c>
     </row>

</xml_diff>